<commit_message>
Updating coverage values for sch
</commit_message>
<xml_diff>
--- a/sch_simulation/data/SCH_params/sch_coverage_scenario_1.xlsx
+++ b/sch_simulation/data/SCH_params/sch_coverage_scenario_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/GitHub/sch/ntd-model-sch/sch_simulation/data/SCH_params/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4FC0BC-1C57-C747-8B88-6F233530FECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC768E5A-F3FA-8049-8671-DCA634AD877F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19200" activeTab="1" xr2:uid="{2B23B0C0-4BFB-41FB-ACE5-EE30D4858695}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19200" xr2:uid="{2B23B0C0-4BFB-41FB-ACE5-EE30D4858695}"/>
   </bookViews>
   <sheets>
     <sheet name="Platform Coverage" sheetId="1" r:id="rId1"/>
@@ -450,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BC57624-070C-4C6C-8EF3-3B0C0B08BDC6}">
   <dimension ref="A1:AD7"/>
   <sheetViews>
-    <sheetView zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -575,40 +575,40 @@
         <v>14</v>
       </c>
       <c r="H2">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="J2">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="L2">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="N2">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="P2">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="R2">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="T2">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="V2">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="X2">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="Z2">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="AB2">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="AD2">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.2">
@@ -720,7 +720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F794004A-4C7C-4E94-81C3-7E7CA0B5D399}">
   <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="181" zoomScaleNormal="181" workbookViewId="0">
+    <sheetView zoomScale="181" zoomScaleNormal="181" workbookViewId="0">
       <selection activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
@@ -972,6 +972,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E3B750AFB9343D42B939C6ACF084A84C" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="93cd09b7eadf1f96f07e4cafc6f5cdf0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00318829-ac19-4fa6-afcb-83e1ad4ea23b" xmlns:ns3="5ffa21b6-e00b-4719-91c3-427b29c2b057" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb8f100d907d4c7940a7c9646b5f1c73" ns2:_="" ns3:_="">
     <xsd:import namespace="00318829-ac19-4fa6-afcb-83e1ad4ea23b"/>
@@ -1188,22 +1203,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6338434B-B586-489B-A269-E3728BE15AC4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E0411F9-2A1E-4488-925A-5AD296329D24}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E6E6D53-A4AA-4BF4-8C61-16B862AC0A51}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1220,21 +1237,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E0411F9-2A1E-4488-925A-5AD296329D24}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6338434B-B586-489B-A269-E3728BE15AC4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>